<commit_message>
Add Database model and update Meeting.xlsx
</commit_message>
<xml_diff>
--- a/Meeting.xlsx
+++ b/Meeting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Listing de toutes les fonctionnalites de l'app</t>
   </si>
@@ -504,7 +504,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -512,7 +514,7 @@
     <col min="2" max="2" width="11.83203125" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" customWidth="1"/>
     <col min="4" max="4" width="1.83203125" customWidth="1"/>
-    <col min="5" max="5" width="43" customWidth="1"/>
+    <col min="5" max="5" width="48.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.5" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="1.6640625" customWidth="1"/>
@@ -670,6 +672,9 @@
       <c r="I10" s="7">
         <v>42295</v>
       </c>
+      <c r="K10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1"/>
@@ -7658,17 +7663,17 @@
     <col min="1" max="1" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>